<commit_message>
gjort en sammanställning av slagljud utan filter
</commit_message>
<xml_diff>
--- a/Testning/Sammanställning.xlsx
+++ b/Testning/Sammanställning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>Test 1</t>
   </si>
@@ -388,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -431,6 +431,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,6 +444,523 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="sv-SE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sv-SE"/>
+              <a:t>Slagljud utan filter</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15043699951518799"/>
+          <c:y val="0.12412256425276653"/>
+          <c:w val="0.60857582292659285"/>
+          <c:h val="0.73942704586740859"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Placering 1 på testbänk</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Blad1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$E$4:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Placering 2 på testbänk</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Blad1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$F$4:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Placering 3 på testbänk</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Blad1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$G$4:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Placering 4 på testbänk</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Blad1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$H$4:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Placering 5 på testbänk</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Blad1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$I$4:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Ej placerbar</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Blad1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$J$4:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="20134528"/>
+        <c:axId val="20165376"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="20134528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sv-SE"/>
+                  <a:t>Var slagljudet</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="sv-SE" baseline="0"/>
+                  <a:t> placerar på testbänken</a:t>
+                </a:r>
+                <a:endParaRPr lang="sv-SE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="20165376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="20165376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sv-SE"/>
+                  <a:t>Antal val</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="sv-SE" baseline="0"/>
+                  <a:t> från testarna</a:t>
+                </a:r>
+                <a:endParaRPr lang="sv-SE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.6985138004246284E-2"/>
+              <c:y val="0.43275928907177452"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="20134528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagram 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -735,7 +1253,7 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S46" sqref="S46"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,9 +1299,7 @@
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="3"/>
       <c r="E3" s="3">
         <v>1</v>
       </c>
@@ -811,12 +1327,18 @@
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="E4" s="6">
+        <v>23</v>
+      </c>
+      <c r="F4" s="6">
+        <v>3</v>
+      </c>
       <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="H4" s="32">
+        <v>1</v>
+      </c>
       <c r="I4" s="7"/>
-      <c r="J4" s="6"/>
+      <c r="J4" s="32"/>
       <c r="P4" s="7"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -828,12 +1350,24 @@
       <c r="D5" s="6">
         <v>2</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="6"/>
+      <c r="E5" s="6">
+        <v>6</v>
+      </c>
+      <c r="F5" s="6">
+        <v>14</v>
+      </c>
+      <c r="G5" s="32">
+        <v>4</v>
+      </c>
+      <c r="H5" s="32">
+        <v>2</v>
+      </c>
+      <c r="I5" s="7">
+        <v>2</v>
+      </c>
+      <c r="J5" s="32">
+        <v>1</v>
+      </c>
       <c r="P5" s="7"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -845,11 +1379,19 @@
       <c r="D6" s="6">
         <v>3</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="E6" s="32">
+        <v>6</v>
+      </c>
+      <c r="F6" s="6">
+        <v>7</v>
+      </c>
+      <c r="G6" s="32">
+        <v>10</v>
+      </c>
       <c r="H6" s="6"/>
-      <c r="I6" s="7"/>
+      <c r="I6" s="7">
+        <v>2</v>
+      </c>
       <c r="J6" s="6"/>
       <c r="P6" s="7"/>
     </row>
@@ -862,11 +1404,21 @@
       <c r="D7" s="6">
         <v>4</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
+      <c r="E7" s="32">
+        <v>2</v>
+      </c>
+      <c r="F7" s="32">
+        <v>3</v>
+      </c>
+      <c r="G7" s="6">
+        <v>6</v>
+      </c>
+      <c r="H7" s="6">
+        <v>13</v>
+      </c>
+      <c r="I7" s="7">
+        <v>4</v>
+      </c>
       <c r="J7" s="6"/>
       <c r="P7" s="7"/>
     </row>
@@ -880,10 +1432,18 @@
         <v>5</v>
       </c>
       <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="10"/>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9">
+        <v>2</v>
+      </c>
+      <c r="H8" s="9">
+        <v>4</v>
+      </c>
+      <c r="I8" s="10">
+        <v>18</v>
+      </c>
       <c r="J8" s="6"/>
       <c r="P8" s="7"/>
     </row>
@@ -1507,6 +2067,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>